<commit_message>
If food is close take the chance
</commit_message>
<xml_diff>
--- a/tests/test_request_move_me_1.xlsx
+++ b/tests/test_request_move_me_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRIOR03\DEV\battle-python\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894B589D-8628-4F5F-9D26-D62A0A4ED01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A694A1-9BDF-4869-9EA3-5D68DDB0036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{CF568A77-CD93-4BC5-8ADF-5BB191CC88ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CF568A77-CD93-4BC5-8ADF-5BB191CC88ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
   <si>
     <t>o</t>
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>Original</t>
   </si>
   <si>
     <t>me</t>
@@ -55,51 +52,6 @@
   </si>
   <si>
     <t>Body</t>
-  </si>
-  <si>
-    <t>All possible</t>
-  </si>
-  <si>
-    <t>without walls</t>
-  </si>
-  <si>
-    <t>without definitely killed</t>
-  </si>
-  <si>
-    <t>Position(x=5, y=5)</t>
-  </si>
-  <si>
-    <t>Position(x=6, y=4)</t>
-  </si>
-  <si>
-    <t>Position(x=4, y=4)</t>
-  </si>
-  <si>
-    <t>Position(x=5, y=9)</t>
-  </si>
-  <si>
-    <t>Position(x=4, y=10)</t>
-  </si>
-  <si>
-    <t>Position(x=4, y=2)</t>
-  </si>
-  <si>
-    <t>Position(x=2, y=5)</t>
-  </si>
-  <si>
-    <t>Position(x=3, y=6)</t>
-  </si>
-  <si>
-    <t>Position(x=1, y=6)</t>
-  </si>
-  <si>
-    <t>Position(x=4, y=6)</t>
-  </si>
-  <si>
-    <t>Position(x=9, y=10)</t>
-  </si>
-  <si>
-    <t>Future Heads</t>
   </si>
 </sst>
 </file>
@@ -536,19 +488,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF189529-94B2-4230-8A83-C7B5B2DC7919}">
-  <dimension ref="A2:O20"/>
+  <dimension ref="A2:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="12" width="5.26953125" customWidth="1"/>
-    <col min="14" max="14" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="5.28515625" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -569,14 +521,9 @@
       <c r="L2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -593,14 +540,9 @@
       <c r="L3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -615,14 +557,9 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="N4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -641,14 +578,9 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="N5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -668,7 +600,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -689,11 +621,9 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="N7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -710,11 +640,8 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="N8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -733,11 +660,8 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-      <c r="N9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -756,11 +680,8 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="N10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -777,11 +698,8 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="N11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -796,11 +714,8 @@
       <c r="J12" s="5"/>
       <c r="K12" s="7"/>
       <c r="L12" s="5"/>
-      <c r="N12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -834,61 +749,31 @@
       <c r="L13">
         <v>10</v>
       </c>
-      <c r="N13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="N14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="N15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
         <v>4</v>
       </c>
-      <c r="N17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>5</v>
-      </c>
-      <c r="N18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="N19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="N20" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>